<commit_message>
small modification in atlas.xlsx
</commit_message>
<xml_diff>
--- a/paper_experiments/docs/atlas.xlsx
+++ b/paper_experiments/docs/atlas.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\boilerad.purdue.edu\cos\userdata\aalsahee\Desktop\USENIX Sec MinRev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aalsahee\ATLAS\paper_experiments\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657E53A4-495E-499E-96FA-8DD8F5D89EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CEF380-A26B-42FA-B1E4-93E1543EF432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B272BCBB-8853-4B72-A4ED-D9E41CEC88A0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Embedding" sheetId="1" r:id="rId1"/>
+    <sheet name="ATLAS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -386,12 +386,24 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -416,9 +428,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,15 +436,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,54 +775,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27" t="s">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="27" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="27" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="35"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="34" t="s">
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="34" t="s">
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="34" t="s">
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="36"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="39"/>
     </row>
     <row r="2" spans="1:29" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -838,14 +838,14 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="24"/>
+      <c r="J2" s="27"/>
       <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
@@ -855,14 +855,14 @@
       <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="23" t="s">
+      <c r="O2" s="27"/>
+      <c r="P2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="24"/>
+      <c r="Q2" s="27"/>
       <c r="R2" s="16" t="s">
         <v>33</v>
       </c>
@@ -887,14 +887,14 @@
       <c r="Y2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" s="33" t="s">
+      <c r="Z2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="23" t="s">
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="AC2" s="24"/>
+      <c r="AC2" s="27"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2054,10 +2054,10 @@
       </c>
     </row>
     <row r="14" spans="1:29" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="37">
+      <c r="B14" s="23">
         <f>E13/(E13+G13)</f>
         <v>0.9039735099337749</v>
       </c>
@@ -2069,10 +2069,10 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="38" t="s">
+      <c r="K14" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="L14" s="37">
+      <c r="L14" s="23">
         <f>N13/(N13+P13)</f>
         <v>0.99888768500161373</v>
       </c>
@@ -2083,10 +2083,10 @@
       <c r="Q14" s="13"/>
     </row>
     <row r="15" spans="1:29" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="23">
         <f>E13/(E13+I13)</f>
         <v>0.97153024911032027</v>
       </c>
@@ -2098,10 +2098,10 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="37">
+      <c r="L15" s="23">
         <f>N13/(N13+Q13)</f>
         <v>0.99949828725649625</v>
       </c>
@@ -2112,10 +2112,10 @@
       <c r="Q15" s="13"/>
     </row>
     <row r="16" spans="1:29" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="37">
+      <c r="B16" s="23">
         <f>2*(R3*S3)/(R3+S3)</f>
         <v>1</v>
       </c>
@@ -2127,10 +2127,10 @@
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
-      <c r="K16" s="38" t="s">
+      <c r="K16" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="L16" s="39">
+      <c r="L16" s="25">
         <f>2*(L14*L15)/(L14+L15)</f>
         <v>0.99919289284499513</v>
       </c>

</xml_diff>